<commit_message>
db and data fixes basic engine settings view
</commit_message>
<xml_diff>
--- a/resources/db.xlsx
+++ b/resources/db.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>Engine</t>
+  </si>
+  <si>
+    <t>6.3-6.1</t>
+  </si>
+  <si>
+    <t>144-139</t>
   </si>
 </sst>
 </file>
@@ -291,7 +297,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -300,7 +306,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -605,7 +610,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -830,6 +835,21 @@
       </c>
     </row>
     <row r="7" spans="2:16">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>1984</v>
+      </c>
+      <c r="F7">
+        <v>140</v>
+      </c>
       <c r="I7">
         <v>3</v>
       </c>
@@ -1090,10 +1110,10 @@
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
       <c r="I17">
         <v>3</v>
       </c>
@@ -1120,10 +1140,10 @@
       </c>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
       <c r="I18">
         <v>3</v>
       </c>
@@ -1150,10 +1170,10 @@
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
       <c r="I19">
         <v>1</v>
       </c>
@@ -1221,7 +1241,30 @@
       <c r="E21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K21" s="8"/>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="J21">
+        <v>4</v>
+      </c>
+      <c r="K21">
+        <v>7</v>
+      </c>
+      <c r="L21">
+        <v>6.9</v>
+      </c>
+      <c r="M21" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" t="s">
+        <v>53</v>
+      </c>
+      <c r="O21">
+        <v>242</v>
+      </c>
+      <c r="P21">
+        <v>42650</v>
+      </c>
     </row>
     <row r="22" spans="1:16">
       <c r="B22">
@@ -1308,34 +1351,43 @@
       </c>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
+      <c r="A28" s="9"/>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28">
+        <v>2018</v>
+      </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="G29" s="9"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
     </row>
     <row r="30" spans="1:16">
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
     </row>
     <row r="31" spans="1:16">
-      <c r="G31" s="10"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="10"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="9"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
     </row>
   </sheetData>
   <sortState ref="H2:Q19">

</xml_diff>

<commit_message>
accessory and paint seed data
</commit_message>
<xml_diff>
--- a/resources/db.xlsx
+++ b/resources/db.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="20115" windowHeight="9030"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="20115" windowHeight="9030" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Engine" sheetId="1" r:id="rId1"/>
+    <sheet name="Accessory" sheetId="2" r:id="rId2"/>
+    <sheet name="Paint" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="140">
   <si>
     <t>ID</t>
   </si>
@@ -283,6 +283,159 @@
   </si>
   <si>
     <t>127-119</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Comfort</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Infotainment</t>
+  </si>
+  <si>
+    <t>Technology and Safety</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Electronic Outside Mirror</t>
+  </si>
+  <si>
+    <t>3 Zone Climate Control</t>
+  </si>
+  <si>
+    <t>Anti Theft Warning System</t>
+  </si>
+  <si>
+    <t>Virtual Cockpit</t>
+  </si>
+  <si>
+    <t>MMI Navigation</t>
+  </si>
+  <si>
+    <t>Audi Sound System</t>
+  </si>
+  <si>
+    <t>Smartphone Interface</t>
+  </si>
+  <si>
+    <t>Assistence-systems</t>
+  </si>
+  <si>
+    <t>Parking Assistant</t>
+  </si>
+  <si>
+    <t>Tour Assistentce Package</t>
+  </si>
+  <si>
+    <t>Pre sense basic</t>
+  </si>
+  <si>
+    <t>Active lane assist</t>
+  </si>
+  <si>
+    <t>Cruise control</t>
+  </si>
+  <si>
+    <t>Head-Up Display</t>
+  </si>
+  <si>
+    <t>Rear view camera</t>
+  </si>
+  <si>
+    <t>Comfort Suspension</t>
+  </si>
+  <si>
+    <t>Sport chassis</t>
+  </si>
+  <si>
+    <t>Side airbags in the back</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>SubCategory</t>
+  </si>
+  <si>
+    <t>Mirror</t>
+  </si>
+  <si>
+    <t>Climate</t>
+  </si>
+  <si>
+    <t>Locksystems</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>Driving and Brakes</t>
+  </si>
+  <si>
+    <t>Uni</t>
+  </si>
+  <si>
+    <t>Metalic</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Pearlescent paint</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>RGB</t>
+  </si>
+  <si>
+    <t>A6AAAD</t>
+  </si>
+  <si>
+    <t>CACFCB</t>
+  </si>
+  <si>
+    <t>161C1C</t>
+  </si>
+  <si>
+    <t>000201</t>
+  </si>
+  <si>
+    <t>434748</t>
+  </si>
+  <si>
+    <t>040203</t>
+  </si>
+  <si>
+    <t>EFEFE7</t>
+  </si>
+  <si>
+    <t>1E281F</t>
   </si>
 </sst>
 </file>
@@ -402,7 +555,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -416,6 +569,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Eingabe" xfId="4" builtinId="20"/>
@@ -716,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37:Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1912,10 +2067,10 @@
       </c>
       <c r="G31" s="9"/>
       <c r="H31" s="10"/>
-      <c r="I31" s="9">
+      <c r="I31">
         <v>9</v>
       </c>
-      <c r="J31" s="9">
+      <c r="J31">
         <v>5</v>
       </c>
       <c r="K31">
@@ -1955,10 +2110,10 @@
       </c>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
-      <c r="I32" s="11">
+      <c r="I32">
         <v>9</v>
       </c>
-      <c r="J32" s="11">
+      <c r="J32">
         <v>5</v>
       </c>
       <c r="K32">
@@ -1984,10 +2139,10 @@
       </c>
     </row>
     <row r="33" spans="9:17">
-      <c r="I33" s="12">
+      <c r="I33">
         <v>9</v>
       </c>
-      <c r="J33" s="11">
+      <c r="J33">
         <v>6</v>
       </c>
       <c r="K33">
@@ -2013,10 +2168,10 @@
       </c>
     </row>
     <row r="34" spans="9:17">
-      <c r="I34" s="12">
+      <c r="I34">
         <v>9</v>
       </c>
-      <c r="J34" s="11">
+      <c r="J34">
         <v>7</v>
       </c>
       <c r="K34">
@@ -2042,10 +2197,10 @@
       </c>
     </row>
     <row r="35" spans="9:17">
-      <c r="I35" s="12">
+      <c r="I35">
         <v>9</v>
       </c>
-      <c r="J35" s="11">
+      <c r="J35">
         <v>6</v>
       </c>
       <c r="K35">
@@ -2071,10 +2226,10 @@
       </c>
     </row>
     <row r="36" spans="9:17">
-      <c r="I36" s="12">
+      <c r="I36">
         <v>9</v>
       </c>
-      <c r="J36" s="11">
+      <c r="J36">
         <v>8</v>
       </c>
       <c r="K36">
@@ -2100,10 +2255,10 @@
       </c>
     </row>
     <row r="37" spans="9:17">
-      <c r="I37" s="12">
+      <c r="I37">
         <v>9</v>
       </c>
-      <c r="J37" s="11">
+      <c r="J37">
         <v>8</v>
       </c>
       <c r="K37">
@@ -2129,31 +2284,31 @@
       </c>
     </row>
     <row r="38" spans="9:17">
-      <c r="I38" s="12">
+      <c r="I38" s="13">
         <v>10</v>
       </c>
-      <c r="J38" s="11">
+      <c r="J38" s="13">
         <v>9</v>
       </c>
-      <c r="K38">
-        <v>7</v>
-      </c>
-      <c r="L38">
+      <c r="K38" s="1">
+        <v>7</v>
+      </c>
+      <c r="L38" s="1">
         <v>10.6</v>
       </c>
-      <c r="M38" t="s">
+      <c r="M38" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="N38" t="s">
+      <c r="N38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="O38">
+      <c r="O38" s="1">
         <v>198</v>
       </c>
-      <c r="P38">
+      <c r="P38" s="1">
         <v>39550</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="Q38" s="1" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2197,24 +2352,519 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F19">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="H27" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="H28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="H29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="H30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="H31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" activeCellId="1" sqref="E11 H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="14">
+        <v>991014</v>
+      </c>
+      <c r="F9">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F10">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11">
+        <v>2400</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more db seed data
</commit_message>
<xml_diff>
--- a/resources/db.xlsx
+++ b/resources/db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="20115" windowHeight="9030" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="20115" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="Engine" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="175">
   <si>
     <t>ID</t>
   </si>
@@ -147,9 +147,6 @@
     <t>121-117</t>
   </si>
   <si>
-    <t>Leistung</t>
-  </si>
-  <si>
     <t>Series</t>
   </si>
   <si>
@@ -436,6 +433,114 @@
   </si>
   <si>
     <t>1E281F</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>Coupe</t>
+  </si>
+  <si>
+    <t>143-137</t>
+  </si>
+  <si>
+    <t>5.9-5.7</t>
+  </si>
+  <si>
+    <t>135-129</t>
+  </si>
+  <si>
+    <t>137-130</t>
+  </si>
+  <si>
+    <t>119-113</t>
+  </si>
+  <si>
+    <t>4.5-4.2</t>
+  </si>
+  <si>
+    <t>119-110</t>
+  </si>
+  <si>
+    <t>138-132</t>
+  </si>
+  <si>
+    <t>126-119</t>
+  </si>
+  <si>
+    <t>5.7-5.4</t>
+  </si>
+  <si>
+    <t>148-141</t>
+  </si>
+  <si>
+    <t>140-138</t>
+  </si>
+  <si>
+    <t>6.1-6.0</t>
+  </si>
+  <si>
+    <t>140-139</t>
+  </si>
+  <si>
+    <t>128-127</t>
+  </si>
+  <si>
+    <t>4.9-4.8</t>
+  </si>
+  <si>
+    <t>128-126</t>
+  </si>
+  <si>
+    <t>5.1-5.3</t>
+  </si>
+  <si>
+    <t>143-140</t>
+  </si>
+  <si>
+    <t>154-148</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>4.7-4.3</t>
+  </si>
+  <si>
+    <t>124-112</t>
+  </si>
+  <si>
+    <t>Leistung (KW)</t>
+  </si>
+  <si>
+    <t>5.8-5.5</t>
+  </si>
+  <si>
+    <t>150-142</t>
+  </si>
+  <si>
+    <t>4.9-4.5</t>
+  </si>
+  <si>
+    <t>129-119</t>
+  </si>
+  <si>
+    <t>155-147</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>127-117</t>
+  </si>
+  <si>
+    <t>5.9-5.6</t>
+  </si>
+  <si>
+    <t>157-148</t>
+  </si>
+  <si>
+    <t>A8</t>
   </si>
 </sst>
 </file>
@@ -555,7 +660,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -569,7 +674,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
@@ -869,23 +973,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37:Q37"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61:S67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="6" width="12" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17">
       <c r="B1" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>6</v>
@@ -905,10 +1010,10 @@
         <v>12</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>43</v>
+        <v>164</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>7</v>
@@ -932,7 +1037,7 @@
         <v>5</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="2:17">
@@ -976,7 +1081,7 @@
         <v>21150</v>
       </c>
       <c r="Q3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="2:17">
@@ -1020,7 +1125,7 @@
         <v>22850</v>
       </c>
       <c r="Q4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="2:17">
@@ -1064,7 +1169,7 @@
         <v>25350</v>
       </c>
       <c r="Q5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="2:17">
@@ -1108,7 +1213,7 @@
         <v>27350</v>
       </c>
       <c r="Q6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="2:17">
@@ -1152,7 +1257,7 @@
         <v>28150</v>
       </c>
       <c r="Q7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="2:17">
@@ -1196,7 +1301,7 @@
         <v>30150</v>
       </c>
       <c r="Q8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="2:17">
@@ -1240,7 +1345,7 @@
         <v>27300</v>
       </c>
       <c r="Q9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="2:17">
@@ -1284,7 +1389,7 @@
         <v>29300</v>
       </c>
       <c r="Q10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="2:17">
@@ -1328,7 +1433,7 @@
         <v>30100</v>
       </c>
       <c r="Q11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="2:17">
@@ -1372,7 +1477,7 @@
         <v>32100</v>
       </c>
       <c r="Q12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="2:17">
@@ -1416,10 +1521,25 @@
         <v>34100</v>
       </c>
       <c r="Q13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:17">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14">
+        <v>2967</v>
+      </c>
+      <c r="F14">
+        <v>210</v>
+      </c>
       <c r="I14">
         <v>4</v>
       </c>
@@ -1445,10 +1565,25 @@
         <v>36100</v>
       </c>
       <c r="Q14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="2:17">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15">
+        <v>1968</v>
+      </c>
+      <c r="F15">
+        <v>150</v>
+      </c>
       <c r="I15">
         <v>2</v>
       </c>
@@ -1474,10 +1609,25 @@
         <v>28350</v>
       </c>
       <c r="Q15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="2:17">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16">
+        <v>2967</v>
+      </c>
+      <c r="F16">
+        <v>170</v>
+      </c>
       <c r="I16">
         <v>2</v>
       </c>
@@ -1503,14 +1653,26 @@
         <v>30350</v>
       </c>
       <c r="Q16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+      <c r="B17" s="9">
+        <v>14</v>
+      </c>
+      <c r="C17" s="9">
+        <v>50</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17">
+        <v>2967</v>
+      </c>
+      <c r="F17">
+        <v>210</v>
+      </c>
       <c r="I17">
         <v>3</v>
       </c>
@@ -1536,7 +1698,7 @@
         <v>31150</v>
       </c>
       <c r="Q17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1569,7 +1731,7 @@
         <v>33150</v>
       </c>
       <c r="Q18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1602,12 +1764,12 @@
         <v>32550</v>
       </c>
       <c r="Q19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="B20" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I20">
         <v>5</v>
@@ -1634,7 +1796,7 @@
         <v>33450</v>
       </c>
       <c r="Q20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1642,10 +1804,10 @@
         <v>0</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>29</v>
@@ -1663,10 +1825,10 @@
         <v>6.9</v>
       </c>
       <c r="M21" t="s">
+        <v>51</v>
+      </c>
+      <c r="N21" t="s">
         <v>52</v>
-      </c>
-      <c r="N21" t="s">
-        <v>53</v>
       </c>
       <c r="O21">
         <v>242</v>
@@ -1675,7 +1837,7 @@
         <v>42650</v>
       </c>
       <c r="Q21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1686,7 +1848,7 @@
         <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22">
         <v>2018</v>
@@ -1704,10 +1866,10 @@
         <v>8.6</v>
       </c>
       <c r="M22" t="s">
+        <v>54</v>
+      </c>
+      <c r="N22" t="s">
         <v>55</v>
-      </c>
-      <c r="N22" t="s">
-        <v>56</v>
       </c>
       <c r="O22">
         <v>224</v>
@@ -1716,7 +1878,7 @@
         <v>32700</v>
       </c>
       <c r="Q22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1727,7 +1889,7 @@
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23">
         <v>2018</v>
@@ -1745,10 +1907,10 @@
         <v>8.9</v>
       </c>
       <c r="M23" t="s">
+        <v>56</v>
+      </c>
+      <c r="N23" t="s">
         <v>57</v>
-      </c>
-      <c r="N23" t="s">
-        <v>58</v>
       </c>
       <c r="O23">
         <v>225</v>
@@ -1757,7 +1919,7 @@
         <v>35000</v>
       </c>
       <c r="Q23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1768,7 +1930,7 @@
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E24">
         <v>2019</v>
@@ -1786,10 +1948,10 @@
         <v>7.2</v>
       </c>
       <c r="M24" t="s">
+        <v>58</v>
+      </c>
+      <c r="N24" t="s">
         <v>59</v>
-      </c>
-      <c r="N24" t="s">
-        <v>60</v>
       </c>
       <c r="O24">
         <v>241</v>
@@ -1798,7 +1960,7 @@
         <v>36800</v>
       </c>
       <c r="Q24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1809,7 +1971,7 @@
         <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25">
         <v>2019</v>
@@ -1830,7 +1992,7 @@
         <v>36</v>
       </c>
       <c r="N25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O25">
         <v>219</v>
@@ -1839,7 +2001,7 @@
         <v>39100</v>
       </c>
       <c r="Q25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1850,7 +2012,7 @@
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26">
         <v>2019</v>
@@ -1868,10 +2030,10 @@
         <v>7.2</v>
       </c>
       <c r="M26" t="s">
+        <v>61</v>
+      </c>
+      <c r="N26" t="s">
         <v>62</v>
-      </c>
-      <c r="N26" t="s">
-        <v>63</v>
       </c>
       <c r="O26">
         <v>241</v>
@@ -1880,7 +2042,7 @@
         <v>39100</v>
       </c>
       <c r="Q26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1891,7 +2053,7 @@
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27">
         <v>2018</v>
@@ -1909,10 +2071,10 @@
         <v>7.7</v>
       </c>
       <c r="M27" t="s">
+        <v>63</v>
+      </c>
+      <c r="N27" t="s">
         <v>64</v>
-      </c>
-      <c r="N27" t="s">
-        <v>65</v>
       </c>
       <c r="O27">
         <v>241</v>
@@ -1921,7 +2083,7 @@
         <v>42150</v>
       </c>
       <c r="Q27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -1933,7 +2095,7 @@
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28">
         <v>2018</v>
@@ -1954,7 +2116,7 @@
         <v>25</v>
       </c>
       <c r="N28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O28">
         <v>235</v>
@@ -1963,7 +2125,7 @@
         <v>44500</v>
       </c>
       <c r="Q28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -1971,10 +2133,10 @@
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E29">
         <v>2019</v>
@@ -1994,10 +2156,10 @@
         <v>10.199999999999999</v>
       </c>
       <c r="M29" t="s">
+        <v>84</v>
+      </c>
+      <c r="N29" t="s">
         <v>85</v>
-      </c>
-      <c r="N29" t="s">
-        <v>86</v>
       </c>
       <c r="O29">
         <v>204</v>
@@ -2006,7 +2168,7 @@
         <v>37700</v>
       </c>
       <c r="Q29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -2014,10 +2176,10 @@
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E30">
         <v>2018</v>
@@ -2037,10 +2199,10 @@
         <v>6.3</v>
       </c>
       <c r="M30" t="s">
+        <v>86</v>
+      </c>
+      <c r="N30" t="s">
         <v>87</v>
-      </c>
-      <c r="N30" t="s">
-        <v>88</v>
       </c>
       <c r="O30">
         <v>250</v>
@@ -2049,7 +2211,7 @@
         <v>47200</v>
       </c>
       <c r="Q30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -2057,10 +2219,10 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E31">
         <v>2019</v>
@@ -2080,10 +2242,10 @@
         <v>8.9</v>
       </c>
       <c r="M31" t="s">
+        <v>70</v>
+      </c>
+      <c r="N31" t="s">
         <v>71</v>
-      </c>
-      <c r="N31" t="s">
-        <v>72</v>
       </c>
       <c r="O31">
         <v>219</v>
@@ -2092,7 +2254,7 @@
         <v>34550</v>
       </c>
       <c r="Q31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -2100,10 +2262,10 @@
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E32">
         <v>2018</v>
@@ -2123,10 +2285,10 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="M32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O32">
         <v>220</v>
@@ -2135,10 +2297,22 @@
         <v>36850</v>
       </c>
       <c r="Q32" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="9:17">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17">
+      <c r="B33" s="1">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33">
+        <v>2018</v>
+      </c>
       <c r="I33">
         <v>9</v>
       </c>
@@ -2152,10 +2326,10 @@
         <v>7.5</v>
       </c>
       <c r="M33" t="s">
+        <v>72</v>
+      </c>
+      <c r="N33" t="s">
         <v>73</v>
-      </c>
-      <c r="N33" t="s">
-        <v>74</v>
       </c>
       <c r="O33">
         <v>236</v>
@@ -2164,10 +2338,22 @@
         <v>38650</v>
       </c>
       <c r="Q33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="9:17">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17">
+      <c r="B34">
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34">
+        <v>2019</v>
+      </c>
       <c r="I34">
         <v>9</v>
       </c>
@@ -2181,10 +2367,10 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="M34" t="s">
+        <v>74</v>
+      </c>
+      <c r="N34" t="s">
         <v>75</v>
-      </c>
-      <c r="N34" t="s">
-        <v>76</v>
       </c>
       <c r="O34">
         <v>213</v>
@@ -2193,10 +2379,22 @@
         <v>40950</v>
       </c>
       <c r="Q34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="9:17">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17">
+      <c r="B35">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35">
+        <v>2018</v>
+      </c>
       <c r="I35">
         <v>9</v>
       </c>
@@ -2210,10 +2408,10 @@
         <v>7.5</v>
       </c>
       <c r="M35" t="s">
+        <v>76</v>
+      </c>
+      <c r="N35" t="s">
         <v>77</v>
-      </c>
-      <c r="N35" t="s">
-        <v>78</v>
       </c>
       <c r="O35">
         <v>236</v>
@@ -2222,10 +2420,22 @@
         <v>40950</v>
       </c>
       <c r="Q35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="9:17">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17">
+      <c r="B36">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36">
+        <v>2019</v>
+      </c>
       <c r="I36">
         <v>9</v>
       </c>
@@ -2239,10 +2449,10 @@
         <v>7.9</v>
       </c>
       <c r="M36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O36">
         <v>231</v>
@@ -2251,10 +2461,22 @@
         <v>44000</v>
       </c>
       <c r="Q36" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="9:17">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17">
+      <c r="B37">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>139</v>
+      </c>
+      <c r="D37" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37">
+        <v>2018</v>
+      </c>
       <c r="I37">
         <v>9</v>
       </c>
@@ -2271,7 +2493,7 @@
         <v>41</v>
       </c>
       <c r="N37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O37">
         <v>230</v>
@@ -2280,39 +2502,63 @@
         <v>46350</v>
       </c>
       <c r="Q37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="9:17">
-      <c r="I38" s="13">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17">
+      <c r="B38">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38">
+        <v>2019</v>
+      </c>
+      <c r="I38">
         <v>10</v>
       </c>
-      <c r="J38" s="13">
+      <c r="J38">
         <v>9</v>
       </c>
-      <c r="K38" s="1">
-        <v>7</v>
-      </c>
-      <c r="L38" s="1">
+      <c r="K38">
+        <v>7</v>
+      </c>
+      <c r="L38">
         <v>10.6</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="M38" t="s">
+        <v>80</v>
+      </c>
+      <c r="N38" t="s">
         <v>81</v>
       </c>
-      <c r="N38" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="O38" s="1">
+      <c r="O38">
         <v>198</v>
       </c>
-      <c r="P38" s="1">
+      <c r="P38">
         <v>39550</v>
       </c>
-      <c r="Q38" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="9:17">
+      <c r="Q38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17">
+      <c r="B39">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>161</v>
+      </c>
+      <c r="D39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39">
+        <v>2019</v>
+      </c>
       <c r="I39" s="12">
         <v>10</v>
       </c>
@@ -2326,10 +2572,10 @@
         <v>6.4</v>
       </c>
       <c r="M39" t="s">
+        <v>82</v>
+      </c>
+      <c r="N39" t="s">
         <v>83</v>
-      </c>
-      <c r="N39" t="s">
-        <v>84</v>
       </c>
       <c r="O39">
         <v>245</v>
@@ -2338,7 +2584,785 @@
         <v>49050</v>
       </c>
       <c r="Q39" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17">
+      <c r="B40">
+        <v>18</v>
+      </c>
+      <c r="C40" t="s">
+        <v>170</v>
+      </c>
+      <c r="D40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40">
+        <v>2019</v>
+      </c>
+      <c r="I40">
+        <v>11</v>
+      </c>
+      <c r="J40">
+        <v>10</v>
+      </c>
+      <c r="K40">
+        <v>7</v>
+      </c>
+      <c r="L40">
+        <v>6.2</v>
+      </c>
+      <c r="M40" t="s">
+        <v>86</v>
+      </c>
+      <c r="N40" t="s">
+        <v>87</v>
+      </c>
+      <c r="O40">
+        <v>250</v>
+      </c>
+      <c r="P40">
+        <v>49900</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17">
+      <c r="B41">
+        <v>19</v>
+      </c>
+      <c r="C41" t="s">
+        <v>174</v>
+      </c>
+      <c r="D41" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41">
+        <v>2019</v>
+      </c>
+      <c r="I41">
+        <v>11</v>
+      </c>
+      <c r="J41">
+        <v>11</v>
+      </c>
+      <c r="K41">
+        <v>8</v>
+      </c>
+      <c r="L41">
+        <v>5.2</v>
+      </c>
+      <c r="M41" t="s">
+        <v>19</v>
+      </c>
+      <c r="N41" t="s">
+        <v>141</v>
+      </c>
+      <c r="O41">
+        <v>250</v>
+      </c>
+      <c r="P41">
+        <v>54550</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17">
+      <c r="I42">
+        <v>12</v>
+      </c>
+      <c r="J42">
+        <v>5</v>
+      </c>
+      <c r="K42">
+        <v>7</v>
+      </c>
+      <c r="L42">
+        <v>9.1</v>
+      </c>
+      <c r="M42" t="s">
+        <v>142</v>
+      </c>
+      <c r="N42" t="s">
+        <v>143</v>
+      </c>
+      <c r="O42">
+        <v>223</v>
+      </c>
+      <c r="P42">
+        <v>38200</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17">
+      <c r="I43">
+        <v>12</v>
+      </c>
+      <c r="J43">
+        <v>6</v>
+      </c>
+      <c r="K43">
+        <v>6</v>
+      </c>
+      <c r="L43">
+        <v>7.5</v>
+      </c>
+      <c r="M43" t="s">
+        <v>54</v>
+      </c>
+      <c r="N43" t="s">
+        <v>144</v>
+      </c>
+      <c r="O43">
+        <v>241</v>
+      </c>
+      <c r="P43">
+        <v>38600</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17">
+      <c r="I44">
+        <v>12</v>
+      </c>
+      <c r="J44">
+        <v>6</v>
+      </c>
+      <c r="K44">
+        <v>7</v>
+      </c>
+      <c r="L44">
+        <v>7.5</v>
+      </c>
+      <c r="M44" t="s">
+        <v>61</v>
+      </c>
+      <c r="N44" t="s">
+        <v>77</v>
+      </c>
+      <c r="O44">
+        <v>241</v>
+      </c>
+      <c r="P44">
+        <v>40900</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17">
+      <c r="I45">
+        <v>12</v>
+      </c>
+      <c r="J45">
+        <v>7</v>
+      </c>
+      <c r="K45">
+        <v>7</v>
+      </c>
+      <c r="L45">
+        <v>9.1</v>
+      </c>
+      <c r="M45" t="s">
+        <v>36</v>
+      </c>
+      <c r="N45" t="s">
+        <v>145</v>
+      </c>
+      <c r="O45">
+        <v>217</v>
+      </c>
+      <c r="P45">
+        <v>41400</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17">
+      <c r="I46">
+        <v>12</v>
+      </c>
+      <c r="J46">
+        <v>8</v>
+      </c>
+      <c r="K46">
+        <v>7</v>
+      </c>
+      <c r="L46">
+        <v>7.9</v>
+      </c>
+      <c r="M46" t="s">
+        <v>146</v>
+      </c>
+      <c r="N46" t="s">
+        <v>147</v>
+      </c>
+      <c r="O46">
+        <v>241</v>
+      </c>
+      <c r="P46">
+        <v>43950</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17">
+      <c r="I47">
+        <v>12</v>
+      </c>
+      <c r="J47">
+        <v>8</v>
+      </c>
+      <c r="K47">
+        <v>7</v>
+      </c>
+      <c r="L47">
+        <v>7.6</v>
+      </c>
+      <c r="M47" t="s">
+        <v>25</v>
+      </c>
+      <c r="N47" t="s">
+        <v>148</v>
+      </c>
+      <c r="O47">
+        <v>235</v>
+      </c>
+      <c r="P47">
+        <v>46300</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17">
+      <c r="I48">
+        <v>13</v>
+      </c>
+      <c r="J48">
+        <v>10</v>
+      </c>
+      <c r="K48">
+        <v>7</v>
+      </c>
+      <c r="L48">
+        <v>6.4</v>
+      </c>
+      <c r="M48" t="s">
+        <v>86</v>
+      </c>
+      <c r="N48" t="s">
+        <v>149</v>
+      </c>
+      <c r="O48">
+        <v>250</v>
+      </c>
+      <c r="P48">
+        <v>49900</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="9:17">
+      <c r="I49">
+        <v>13</v>
+      </c>
+      <c r="J49">
+        <v>11</v>
+      </c>
+      <c r="K49">
+        <v>8</v>
+      </c>
+      <c r="L49">
+        <v>5.3</v>
+      </c>
+      <c r="M49" t="s">
+        <v>150</v>
+      </c>
+      <c r="N49" t="s">
+        <v>151</v>
+      </c>
+      <c r="O49">
+        <v>250</v>
+      </c>
+      <c r="P49">
+        <v>54550</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="9:17">
+      <c r="I50">
+        <v>14</v>
+      </c>
+      <c r="J50">
+        <v>6</v>
+      </c>
+      <c r="K50">
+        <v>6</v>
+      </c>
+      <c r="L50">
+        <v>7.9</v>
+      </c>
+      <c r="M50">
+        <v>6.1</v>
+      </c>
+      <c r="N50" t="s">
+        <v>152</v>
+      </c>
+      <c r="O50">
+        <v>241</v>
+      </c>
+      <c r="P50">
+        <v>46500</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="9:17">
+      <c r="I51">
+        <v>14</v>
+      </c>
+      <c r="J51">
+        <v>6</v>
+      </c>
+      <c r="K51">
+        <v>7</v>
+      </c>
+      <c r="L51">
+        <v>7.9</v>
+      </c>
+      <c r="M51" t="s">
+        <v>153</v>
+      </c>
+      <c r="N51" t="s">
+        <v>154</v>
+      </c>
+      <c r="O51">
+        <v>241</v>
+      </c>
+      <c r="P51">
+        <v>48800</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="9:17">
+      <c r="I52">
+        <v>14</v>
+      </c>
+      <c r="J52">
+        <v>7</v>
+      </c>
+      <c r="K52">
+        <v>7</v>
+      </c>
+      <c r="L52">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="M52">
+        <v>4.8</v>
+      </c>
+      <c r="N52" t="s">
+        <v>155</v>
+      </c>
+      <c r="O52">
+        <v>213</v>
+      </c>
+      <c r="P52">
+        <v>49300</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="9:17">
+      <c r="I53">
+        <v>14</v>
+      </c>
+      <c r="J53">
+        <v>8</v>
+      </c>
+      <c r="K53">
+        <v>7</v>
+      </c>
+      <c r="L53">
+        <v>8.4</v>
+      </c>
+      <c r="M53" t="s">
+        <v>156</v>
+      </c>
+      <c r="N53" t="s">
+        <v>157</v>
+      </c>
+      <c r="O53">
+        <v>241</v>
+      </c>
+      <c r="P53">
+        <v>51850</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="9:17">
+      <c r="I54">
+        <v>14</v>
+      </c>
+      <c r="J54">
+        <v>8</v>
+      </c>
+      <c r="K54">
+        <v>7</v>
+      </c>
+      <c r="L54">
+        <v>8</v>
+      </c>
+      <c r="M54" t="s">
+        <v>158</v>
+      </c>
+      <c r="N54" t="s">
+        <v>159</v>
+      </c>
+      <c r="O54">
+        <v>233</v>
+      </c>
+      <c r="P54">
+        <v>54200</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="9:17">
+      <c r="I55">
+        <v>15</v>
+      </c>
+      <c r="J55">
+        <v>11</v>
+      </c>
+      <c r="K55">
+        <v>8</v>
+      </c>
+      <c r="L55">
+        <v>5.7</v>
+      </c>
+      <c r="M55" t="s">
+        <v>142</v>
+      </c>
+      <c r="N55" t="s">
+        <v>160</v>
+      </c>
+      <c r="O55">
+        <v>250</v>
+      </c>
+      <c r="P55">
+        <v>60750</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="9:17">
+      <c r="I56">
+        <v>16</v>
+      </c>
+      <c r="J56">
+        <v>12</v>
+      </c>
+      <c r="K56">
+        <v>7</v>
+      </c>
+      <c r="L56">
+        <v>8.1</v>
+      </c>
+      <c r="M56" t="s">
+        <v>162</v>
+      </c>
+      <c r="N56" t="s">
+        <v>163</v>
+      </c>
+      <c r="O56">
+        <v>246</v>
+      </c>
+      <c r="P56">
+        <v>49150</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="9:17">
+      <c r="I57">
+        <v>16</v>
+      </c>
+      <c r="J57">
+        <v>13</v>
+      </c>
+      <c r="K57">
+        <v>8</v>
+      </c>
+      <c r="L57">
+        <v>6.3</v>
+      </c>
+      <c r="M57" t="s">
+        <v>165</v>
+      </c>
+      <c r="N57" t="s">
+        <v>166</v>
+      </c>
+      <c r="O57">
+        <v>250</v>
+      </c>
+      <c r="P57">
+        <v>55050</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="9:17">
+      <c r="I58">
+        <v>16</v>
+      </c>
+      <c r="J58">
+        <v>14</v>
+      </c>
+      <c r="K58">
+        <v>8</v>
+      </c>
+      <c r="L58">
+        <v>5.5</v>
+      </c>
+      <c r="M58" t="s">
+        <v>165</v>
+      </c>
+      <c r="N58" t="s">
+        <v>166</v>
+      </c>
+      <c r="O58">
+        <v>250</v>
+      </c>
+      <c r="P58">
+        <v>58050</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="9:17">
+      <c r="I59">
+        <v>17</v>
+      </c>
+      <c r="J59">
+        <v>12</v>
+      </c>
+      <c r="K59">
+        <v>7</v>
+      </c>
+      <c r="L59">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="M59" t="s">
+        <v>167</v>
+      </c>
+      <c r="N59" t="s">
+        <v>168</v>
+      </c>
+      <c r="O59">
+        <v>241</v>
+      </c>
+      <c r="P59">
+        <v>53950</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="9:17">
+      <c r="I60">
+        <v>17</v>
+      </c>
+      <c r="J60">
+        <v>13</v>
+      </c>
+      <c r="K60">
+        <v>8</v>
+      </c>
+      <c r="L60">
+        <v>6.5</v>
+      </c>
+      <c r="M60" t="s">
+        <v>142</v>
+      </c>
+      <c r="N60" t="s">
+        <v>169</v>
+      </c>
+      <c r="O60">
+        <v>250</v>
+      </c>
+      <c r="P60">
+        <v>59850</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="9:17">
+      <c r="I61">
+        <v>17</v>
+      </c>
+      <c r="J61">
+        <v>14</v>
+      </c>
+      <c r="K61">
+        <v>8</v>
+      </c>
+      <c r="L61">
+        <v>5.7</v>
+      </c>
+      <c r="M61" t="s">
+        <v>142</v>
+      </c>
+      <c r="N61" t="s">
+        <v>169</v>
+      </c>
+      <c r="O61">
+        <v>250</v>
+      </c>
+      <c r="P61">
+        <v>62850</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="9:17">
+      <c r="I62">
+        <v>18</v>
+      </c>
+      <c r="J62">
+        <v>12</v>
+      </c>
+      <c r="K62">
+        <v>7</v>
+      </c>
+      <c r="L62">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="M62" t="s">
+        <v>167</v>
+      </c>
+      <c r="N62" t="s">
+        <v>171</v>
+      </c>
+      <c r="O62">
+        <v>245</v>
+      </c>
+      <c r="P62">
+        <v>57500</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="9:17">
+      <c r="I63">
+        <v>18</v>
+      </c>
+      <c r="J63">
+        <v>13</v>
+      </c>
+      <c r="K63">
+        <v>8</v>
+      </c>
+      <c r="L63">
+        <v>6.5</v>
+      </c>
+      <c r="M63" t="s">
+        <v>165</v>
+      </c>
+      <c r="N63" t="s">
+        <v>166</v>
+      </c>
+      <c r="O63">
+        <v>250</v>
+      </c>
+      <c r="P63">
+        <v>62900</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="9:17">
+      <c r="I64">
+        <v>18</v>
+      </c>
+      <c r="J64">
+        <v>14</v>
+      </c>
+      <c r="K64">
+        <v>8</v>
+      </c>
+      <c r="L64">
+        <v>5.7</v>
+      </c>
+      <c r="M64" t="s">
+        <v>165</v>
+      </c>
+      <c r="N64" t="s">
+        <v>166</v>
+      </c>
+      <c r="O64">
+        <v>250</v>
+      </c>
+      <c r="P64">
+        <v>66300</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="9:17">
+      <c r="I65">
+        <v>19</v>
+      </c>
+      <c r="J65">
+        <v>14</v>
+      </c>
+      <c r="K65">
+        <v>8</v>
+      </c>
+      <c r="L65">
+        <v>5.9</v>
+      </c>
+      <c r="M65" t="s">
+        <v>172</v>
+      </c>
+      <c r="N65" t="s">
+        <v>173</v>
+      </c>
+      <c r="O65">
+        <v>250</v>
+      </c>
+      <c r="P65">
+        <v>91900</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2372,16 +3396,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="G2" s="5"/>
     </row>
@@ -2390,13 +3414,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3">
         <v>345</v>
@@ -2407,13 +3431,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F4">
         <v>695</v>
@@ -2424,13 +3448,13 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F5">
         <v>480</v>
@@ -2441,13 +3465,13 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6">
         <v>500</v>
@@ -2458,13 +3482,13 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F7">
         <v>1500</v>
@@ -2475,13 +3499,13 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8">
         <v>290</v>
@@ -2492,13 +3516,13 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F9">
         <v>400</v>
@@ -2509,10 +3533,10 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" t="s">
         <v>103</v>
-      </c>
-      <c r="E10" t="s">
-        <v>104</v>
       </c>
       <c r="F10">
         <v>1750</v>
@@ -2523,10 +3547,10 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F11">
         <v>1640</v>
@@ -2537,10 +3561,10 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F12">
         <v>250</v>
@@ -2551,10 +3575,10 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F13">
         <v>600</v>
@@ -2565,10 +3589,10 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F14">
         <v>300</v>
@@ -2579,10 +3603,10 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F15">
         <v>980</v>
@@ -2593,10 +3617,10 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F16">
         <v>450</v>
@@ -2607,13 +3631,13 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F17">
         <v>980</v>
@@ -2624,13 +3648,13 @@
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F18">
         <v>340</v>
@@ -2641,10 +3665,10 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F19">
         <v>360</v>
@@ -2652,27 +3676,27 @@
     </row>
     <row r="27" spans="2:8">
       <c r="H27" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="2:8">
       <c r="H28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="2:8">
       <c r="H29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="2:8">
       <c r="H30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="2:8">
       <c r="H31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2685,7 +3709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" activeCellId="1" sqref="E11 H11"/>
     </sheetView>
   </sheetViews>
@@ -2699,16 +3723,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="2:6">
@@ -2716,13 +3740,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>137</v>
+        <v>114</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>136</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2733,13 +3757,13 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>138</v>
+        <v>115</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -2750,13 +3774,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" t="s">
         <v>125</v>
       </c>
-      <c r="D5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>132</v>
+      <c r="E5" s="13" t="s">
+        <v>131</v>
       </c>
       <c r="F5">
         <v>900</v>
@@ -2767,13 +3791,13 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>133</v>
+        <v>115</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>132</v>
       </c>
       <c r="F6">
         <v>900</v>
@@ -2784,13 +3808,13 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>134</v>
+        <v>126</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>133</v>
       </c>
       <c r="F7">
         <v>900</v>
@@ -2801,13 +3825,13 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>135</v>
+        <v>114</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>134</v>
       </c>
       <c r="F8">
         <v>900</v>
@@ -2818,12 +3842,12 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="14">
+        <v>127</v>
+      </c>
+      <c r="E9" s="13">
         <v>991014</v>
       </c>
       <c r="F9">
@@ -2835,13 +3859,13 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>136</v>
+        <v>126</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="F10">
         <v>2400</v>
@@ -2852,13 +3876,13 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" t="s">
         <v>129</v>
       </c>
-      <c r="D11" t="s">
-        <v>130</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>139</v>
+      <c r="E11" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="F11">
         <v>2400</v>

</xml_diff>

<commit_message>
db categories as entities
</commit_message>
<xml_diff>
--- a/resources/db.xlsx
+++ b/resources/db.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="20115" windowHeight="9030"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="20115" windowHeight="9030" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Engine" sheetId="1" r:id="rId1"/>
     <sheet name="Accessory" sheetId="2" r:id="rId2"/>
     <sheet name="Paint" sheetId="3" r:id="rId3"/>
+    <sheet name="Rims" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="176">
   <si>
     <t>ID</t>
   </si>
@@ -541,6 +542,9 @@
   </si>
   <si>
     <t>A8</t>
+  </si>
+  <si>
+    <t>Size</t>
   </si>
 </sst>
 </file>
@@ -660,7 +664,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -675,6 +679,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Eingabe" xfId="4" builtinId="20"/>
@@ -975,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61:S67"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1036,7 +1041,7 @@
       <c r="P2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="14" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3707,18 +3712,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F11"/>
+  <dimension ref="B2:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" activeCellId="1" sqref="E11 H11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:7">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -3735,9 +3741,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:7">
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>123</v>
@@ -3752,9 +3758,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:7">
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>123</v>
@@ -3769,9 +3775,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:7">
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>124</v>
@@ -3786,9 +3792,9 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:7">
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>124</v>
@@ -3803,9 +3809,9 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:7">
       <c r="B7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>124</v>
@@ -3820,9 +3826,9 @@
         <v>900</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:7">
       <c r="B8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>124</v>
@@ -3837,9 +3843,9 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:7">
       <c r="B9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
         <v>124</v>
@@ -3854,9 +3860,9 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:7">
       <c r="B10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
         <v>128</v>
@@ -3871,9 +3877,9 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:7">
       <c r="B11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
         <v>128</v>
@@ -3885,6 +3891,98 @@
         <v>138</v>
       </c>
       <c r="F11">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="G15" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="G16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7">
+      <c r="G17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7">
+      <c r="G18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="2:5">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>19</v>
+      </c>
+      <c r="D6">
         <v>2400</v>
       </c>
     </row>

</xml_diff>